<commit_message>
Add Meta Baumann Type
</commit_message>
<xml_diff>
--- a/survey_question_to_db/answer_weight.xlsx
+++ b/survey_question_to_db/answer_weight.xlsx
@@ -513,7 +513,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="inlineStr"/>
       <c r="E4" t="inlineStr"/>
@@ -527,7 +527,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
         <v>2</v>
@@ -1098,9 +1098,7 @@
         <v>4</v>
       </c>
       <c r="H42" t="inlineStr"/>
-      <c r="I42" t="n">
-        <v>4</v>
-      </c>
+      <c r="I42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -1115,9 +1113,7 @@
         <v>2</v>
       </c>
       <c r="H43" t="inlineStr"/>
-      <c r="I43" t="n">
-        <v>2</v>
-      </c>
+      <c r="I43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -1131,9 +1127,7 @@
         <v>2</v>
       </c>
       <c r="G44" t="inlineStr"/>
-      <c r="H44" t="n">
-        <v>2</v>
-      </c>
+      <c r="H44" t="inlineStr"/>
       <c r="I44" t="inlineStr"/>
     </row>
     <row r="45">
@@ -1148,9 +1142,7 @@
         <v>4</v>
       </c>
       <c r="G45" t="inlineStr"/>
-      <c r="H45" t="n">
-        <v>4</v>
-      </c>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="inlineStr"/>
     </row>
     <row r="46">

</xml_diff>